<commit_message>
Update Fitness Vision 2022 cf v1-0 170522.xlsx
</commit_message>
<xml_diff>
--- a/Fitness Vision 2022 cf v1-0 170522.xlsx
+++ b/Fitness Vision 2022 cf v1-0 170522.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6C14DD34-1FD5-4924-91B1-56E7D69F27C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A683C0-7B95-4F80-A725-9F8EB8468BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fitness Vision" sheetId="2" r:id="rId1"/>
     <sheet name="Directions" sheetId="1" r:id="rId2"/>
+    <sheet name="Command Lines" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -8407,7 +8408,7 @@
   </sheetPr>
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -8694,6 +8695,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3402AC53-B45C-44C0-8B5E-4D28D12E5346}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a754d229f0057affa62b555f2ac55d44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c067517bd06b16cb9c9e315ad40fb255" ns2:_="" ns3:_="">
@@ -8916,21 +8929,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
     <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8953,6 +8966,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D2BA575-B720-47A2-8DBB-E6F83249DCD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55EC2C68-DDBE-4CEA-B267-5802E87CBD15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8960,12 +8981,4 @@
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D2BA575-B720-47A2-8DBB-E6F83249DCD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>